<commit_message>
we go. Hard 추가
</commit_message>
<xml_diff>
--- a/NoteMaps/WeGo_Fromis9.xlsx
+++ b/NoteMaps/WeGo_Fromis9.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eogus\source\repos\RhythmGame\NoteMaps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB3B400-319C-4468-9E4A-27EA5627F3FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F8170791-E6B6-4066-8090-E93717ECE6A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FBD1AADC-AD03-4139-A607-30D499883534}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="WeGo_Fromis9" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{597C38B7-F2CF-4951-BED7-7D28309F5979}">
   <dimension ref="A1:G1255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1021" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G740" sqref="G740"/>
+    <sheetView tabSelected="1" topLeftCell="A1212" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="S1227" sqref="S1227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -5806,8 +5806,8 @@
       <c r="C236" s="2">
         <v>5</v>
       </c>
-      <c r="D236" s="1">
-        <v>1</v>
+      <c r="D236">
+        <v>0</v>
       </c>
       <c r="E236">
         <v>0</v>
@@ -5855,8 +5855,8 @@
       <c r="D238">
         <v>0</v>
       </c>
-      <c r="E238" s="1">
-        <v>1</v>
+      <c r="E238">
+        <v>0</v>
       </c>
       <c r="F238">
         <v>0</v>
@@ -6778,8 +6778,8 @@
       <c r="E278">
         <v>0</v>
       </c>
-      <c r="F278">
-        <v>0</v>
+      <c r="F278" s="1">
+        <v>1</v>
       </c>
       <c r="G278">
         <v>0</v>
@@ -7379,8 +7379,8 @@
       <c r="F304">
         <v>0</v>
       </c>
-      <c r="G304">
-        <v>0</v>
+      <c r="G304" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="305" spans="1:7" x14ac:dyDescent="0.4">
@@ -7511,8 +7511,8 @@
       <c r="D310">
         <v>0</v>
       </c>
-      <c r="E310">
-        <v>0</v>
+      <c r="E310" s="1">
+        <v>1</v>
       </c>
       <c r="F310">
         <v>0</v>
@@ -8112,8 +8112,8 @@
       <c r="E336">
         <v>0</v>
       </c>
-      <c r="F336">
-        <v>0</v>
+      <c r="F336" s="1">
+        <v>1</v>
       </c>
       <c r="G336">
         <v>0</v>
@@ -8664,11 +8664,11 @@
       <c r="E360">
         <v>0</v>
       </c>
-      <c r="F360" s="1">
-        <v>1</v>
-      </c>
-      <c r="G360">
-        <v>0</v>
+      <c r="F360">
+        <v>0</v>
+      </c>
+      <c r="G360" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="361" spans="1:7" x14ac:dyDescent="0.4">
@@ -8710,8 +8710,8 @@
       <c r="E362">
         <v>0</v>
       </c>
-      <c r="F362">
-        <v>0</v>
+      <c r="F362" s="1">
+        <v>1</v>
       </c>
       <c r="G362">
         <v>0</v>
@@ -8805,8 +8805,8 @@
       <c r="F366">
         <v>0</v>
       </c>
-      <c r="G366" s="1">
-        <v>1</v>
+      <c r="G366">
+        <v>0</v>
       </c>
     </row>
     <row r="367" spans="1:7" x14ac:dyDescent="0.4">
@@ -8848,11 +8848,11 @@
       <c r="E368">
         <v>0</v>
       </c>
-      <c r="F368" s="1">
-        <v>1</v>
-      </c>
-      <c r="G368">
-        <v>0</v>
+      <c r="F368">
+        <v>0</v>
+      </c>
+      <c r="G368" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="369" spans="1:7" x14ac:dyDescent="0.4">
@@ -8894,8 +8894,8 @@
       <c r="E370">
         <v>0</v>
       </c>
-      <c r="F370">
-        <v>0</v>
+      <c r="F370" s="1">
+        <v>1</v>
       </c>
       <c r="G370">
         <v>0</v>
@@ -8989,8 +8989,8 @@
       <c r="F374">
         <v>0</v>
       </c>
-      <c r="G374" s="1">
-        <v>1</v>
+      <c r="G374">
+        <v>0</v>
       </c>
     </row>
     <row r="375" spans="1:7" x14ac:dyDescent="0.4">
@@ -9032,11 +9032,11 @@
       <c r="E376">
         <v>0</v>
       </c>
-      <c r="F376" s="1">
-        <v>1</v>
-      </c>
-      <c r="G376">
-        <v>0</v>
+      <c r="F376">
+        <v>0</v>
+      </c>
+      <c r="G376" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="377" spans="1:7" x14ac:dyDescent="0.4">
@@ -9078,8 +9078,8 @@
       <c r="E378">
         <v>0</v>
       </c>
-      <c r="F378">
-        <v>0</v>
+      <c r="F378" s="1">
+        <v>1</v>
       </c>
       <c r="G378">
         <v>0</v>
@@ -9173,8 +9173,8 @@
       <c r="F382">
         <v>0</v>
       </c>
-      <c r="G382" s="1">
-        <v>1</v>
+      <c r="G382">
+        <v>0</v>
       </c>
     </row>
     <row r="383" spans="1:7" x14ac:dyDescent="0.4">
@@ -10504,8 +10504,8 @@
       <c r="E440" s="1">
         <v>1</v>
       </c>
-      <c r="F440">
-        <v>0</v>
+      <c r="F440" s="1">
+        <v>1</v>
       </c>
       <c r="G440">
         <v>0</v>
@@ -10685,8 +10685,8 @@
       <c r="D448" s="1">
         <v>1</v>
       </c>
-      <c r="E448">
-        <v>0</v>
+      <c r="E448" s="1">
+        <v>1</v>
       </c>
       <c r="F448">
         <v>0</v>
@@ -11240,8 +11240,8 @@
       <c r="E472" s="1">
         <v>1</v>
       </c>
-      <c r="F472">
-        <v>0</v>
+      <c r="F472" s="1">
+        <v>1</v>
       </c>
       <c r="G472">
         <v>0</v>
@@ -11421,8 +11421,8 @@
       <c r="D480" s="1">
         <v>1</v>
       </c>
-      <c r="E480">
-        <v>0</v>
+      <c r="E480" s="1">
+        <v>1</v>
       </c>
       <c r="F480">
         <v>0</v>
@@ -11608,8 +11608,8 @@
       <c r="E488">
         <v>0</v>
       </c>
-      <c r="F488">
-        <v>0</v>
+      <c r="F488" s="1">
+        <v>1</v>
       </c>
       <c r="G488" s="1">
         <v>1</v>
@@ -11700,11 +11700,11 @@
       <c r="E492">
         <v>0</v>
       </c>
-      <c r="F492">
-        <v>0</v>
-      </c>
-      <c r="G492" s="1">
-        <v>1</v>
+      <c r="F492" s="1">
+        <v>1</v>
+      </c>
+      <c r="G492">
+        <v>0</v>
       </c>
     </row>
     <row r="493" spans="1:7" x14ac:dyDescent="0.4">
@@ -11789,8 +11789,8 @@
       <c r="D496">
         <v>0</v>
       </c>
-      <c r="E496">
-        <v>0</v>
+      <c r="E496" s="1">
+        <v>1</v>
       </c>
       <c r="F496" s="1">
         <v>1</v>
@@ -11881,11 +11881,11 @@
       <c r="D500">
         <v>0</v>
       </c>
-      <c r="E500">
-        <v>0</v>
-      </c>
-      <c r="F500" s="1">
-        <v>1</v>
+      <c r="E500" s="1">
+        <v>1</v>
+      </c>
+      <c r="F500">
+        <v>0</v>
       </c>
       <c r="G500">
         <v>0</v>
@@ -12301,8 +12301,8 @@
       <c r="F518">
         <v>0</v>
       </c>
-      <c r="G518">
-        <v>0</v>
+      <c r="G518" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="519" spans="1:7" x14ac:dyDescent="0.4">
@@ -12344,8 +12344,8 @@
       <c r="E520">
         <v>0</v>
       </c>
-      <c r="F520">
-        <v>0</v>
+      <c r="F520" s="1">
+        <v>1</v>
       </c>
       <c r="G520">
         <v>0</v>
@@ -15006,14 +15006,14 @@
       <c r="C636" s="2">
         <v>5</v>
       </c>
-      <c r="D636">
-        <v>0</v>
+      <c r="D636" s="1">
+        <v>1</v>
       </c>
       <c r="E636">
         <v>0</v>
       </c>
-      <c r="F636" s="1">
-        <v>1</v>
+      <c r="F636">
+        <v>0</v>
       </c>
       <c r="G636">
         <v>0</v>
@@ -15104,11 +15104,11 @@
       <c r="E640">
         <v>0</v>
       </c>
-      <c r="F640">
-        <v>0</v>
-      </c>
-      <c r="G640" s="1">
-        <v>1</v>
+      <c r="F640" s="1">
+        <v>1</v>
+      </c>
+      <c r="G640">
+        <v>0</v>
       </c>
     </row>
     <row r="641" spans="1:7" x14ac:dyDescent="0.4">
@@ -15193,14 +15193,14 @@
       <c r="D644">
         <v>0</v>
       </c>
-      <c r="E644">
-        <v>0</v>
+      <c r="E644" s="1">
+        <v>1</v>
       </c>
       <c r="F644">
         <v>0</v>
       </c>
-      <c r="G644" s="1">
-        <v>1</v>
+      <c r="G644">
+        <v>0</v>
       </c>
     </row>
     <row r="645" spans="1:7" x14ac:dyDescent="0.4">
@@ -15374,14 +15374,14 @@
       <c r="C652" s="2">
         <v>5</v>
       </c>
-      <c r="D652">
-        <v>0</v>
+      <c r="D652" s="1">
+        <v>1</v>
       </c>
       <c r="E652">
         <v>0</v>
       </c>
-      <c r="F652" s="1">
-        <v>1</v>
+      <c r="F652">
+        <v>0</v>
       </c>
       <c r="G652">
         <v>0</v>
@@ -15423,8 +15423,8 @@
       <c r="D654">
         <v>0</v>
       </c>
-      <c r="E654">
-        <v>0</v>
+      <c r="E654" s="1">
+        <v>1</v>
       </c>
       <c r="F654">
         <v>0</v>
@@ -15466,8 +15466,8 @@
       <c r="C656" s="2">
         <v>1</v>
       </c>
-      <c r="D656">
-        <v>0</v>
+      <c r="D656" s="1">
+        <v>1</v>
       </c>
       <c r="E656">
         <v>0</v>
@@ -18824,8 +18824,8 @@
       <c r="C802" s="2">
         <v>3</v>
       </c>
-      <c r="D802" s="1">
-        <v>1</v>
+      <c r="D802">
+        <v>0</v>
       </c>
       <c r="E802">
         <v>0</v>
@@ -18870,8 +18870,8 @@
       <c r="C804" s="2">
         <v>5</v>
       </c>
-      <c r="D804">
-        <v>0</v>
+      <c r="D804" s="1">
+        <v>1</v>
       </c>
       <c r="E804">
         <v>0</v>
@@ -21679,8 +21679,8 @@
       <c r="D926">
         <v>0</v>
       </c>
-      <c r="E926" s="1">
-        <v>1</v>
+      <c r="E926">
+        <v>0</v>
       </c>
       <c r="F926">
         <v>0</v>
@@ -21725,8 +21725,8 @@
       <c r="D928">
         <v>0</v>
       </c>
-      <c r="E928">
-        <v>0</v>
+      <c r="E928" s="1">
+        <v>1</v>
       </c>
       <c r="F928">
         <v>0</v>
@@ -27567,8 +27567,8 @@
       <c r="D1182">
         <v>0</v>
       </c>
-      <c r="E1182" s="1">
-        <v>1</v>
+      <c r="E1182">
+        <v>0</v>
       </c>
       <c r="F1182">
         <v>0</v>
@@ -27613,8 +27613,8 @@
       <c r="D1184">
         <v>0</v>
       </c>
-      <c r="E1184">
-        <v>0</v>
+      <c r="E1184" s="1">
+        <v>1</v>
       </c>
       <c r="F1184">
         <v>0</v>

</xml_diff>